<commit_message>
Pushing Bob's latest SNS changes
</commit_message>
<xml_diff>
--- a/source/_docs/AWS Error Codes.xlsx
+++ b/source/_docs/AWS Error Codes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>Code</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>NoSuchKey - The specified key does not exist.</t>
+  </si>
+  <si>
+    <t>NoSuchVersion - The version ID specified in the request does not match an existing version.</t>
+  </si>
+  <si>
+    <t>NotImplemented - A provided header implies functionality that is not implemented.</t>
   </si>
 </sst>
 </file>
@@ -474,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,6 +783,28 @@
         <v>29</v>
       </c>
     </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>412025</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>412026</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>